<commit_message>
Agregado a precondicion:"Que existan oportunidades asignadas a telemarketers".
</commit_message>
<xml_diff>
--- a/CU1.2 Ver Oportunidad.xlsx
+++ b/CU1.2 Ver Oportunidad.xlsx
@@ -79,10 +79,11 @@
     <t>Caso de Uso</t>
   </si>
   <si>
-    <t>Que el actor tenga los permisos necesarios para ver el registro.</t>
-  </si>
-  <si>
     <t>El actor hace clic en el botón "Ver" en algún registro del listado de oportunidades</t>
+  </si>
+  <si>
+    <t>Que el actor tenga los permisos necesarios para ver el registro.
+Que existan oportunidades asignadas a telemarketers.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +545,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,12 +624,12 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -651,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10"/>
     </row>

</xml_diff>

<commit_message>
Modifiaciones: -Descripción -Actores -Precondición
</commit_message>
<xml_diff>
--- a/CU1.2 Ver Oportunidad.xlsx
+++ b/CU1.2 Ver Oportunidad.xlsx
@@ -37,15 +37,9 @@
     <t>Pre-condición</t>
   </si>
   <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
     <t>Actores</t>
   </si>
   <si>
-    <t>Se muestran en pantalla todos los datos de la oportunidad seleccionada.</t>
-  </si>
-  <si>
     <t>Descripción</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>Versión</t>
   </si>
   <si>
@@ -83,7 +74,17 @@
   </si>
   <si>
     <t>Que el actor tenga los permisos necesarios para ver el registro.
+Que existan oportunidades en estado "Abierta"
 Que existan oportunidades asignadas a telemarketers.</t>
+  </si>
+  <si>
+    <t>Se muestran en pantalla todos los datos de la oportunidad seleccionada incluyendo en la esquina inferior derecha el botón "Llamar".</t>
+  </si>
+  <si>
+    <t>Coordinador/Supervisor/Telemarketer</t>
+  </si>
+  <si>
+    <t>0003</t>
   </si>
 </sst>
 </file>
@@ -545,7 +546,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +558,7 @@
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="16">
         <v>42890</v>
@@ -565,71 +566,71 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -652,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="10"/>
     </row>

</xml_diff>